<commit_message>
Added Test Plan PDF
Created PDF version of Text Plan spreadsheet.
</commit_message>
<xml_diff>
--- a/Testing/Test Plan.xlsx
+++ b/Testing/Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fined\Google Drive\School\Capstone\CherokeeLanguageStudyTool\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDFDD5F-A1F8-4F0E-A9CC-657402002230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1679BF27-2733-4E7C-91A0-A8A08F2E6435}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41172" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="8" xr2:uid="{1C392581-7671-438D-9252-DC5D3E4BE7A7}"/>
+    <workbookView xWindow="41172" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="1" activeTab="2" xr2:uid="{1C392581-7671-438D-9252-DC5D3E4BE7A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Menu" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,98 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="30">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -517,6 +608,159 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{99C83D3A-77FB-43A1-B018-67545DEF22CF}" name="Table1" displayName="Table1" ref="A1:H16" totalsRowShown="0" dataDxfId="24">
+  <autoFilter ref="A1:H16" xr:uid="{6AE1E8D1-CD45-4947-B94A-4E2AD3CE6525}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D8A388C3-C877-4952-A1F7-46F9E5EA082B}" name="Task"/>
+    <tableColumn id="2" xr3:uid="{AE18E612-EA14-4B02-A775-9C263085B842}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{088FFB44-E63E-4AEE-AD1E-554D87C008F1}" name="Expectation" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{43D3140C-6096-46C7-AE33-51A9C059F3EA}" name="Working Initially on Installable?" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{BBA136CD-4D21-4944-8FC5-DB45287B0B26}" name="Working Initially on Standalone?" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{ED43473A-3B7B-4A47-A871-1549471D01BA}" name="Issue" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{A11B3361-0701-4BB9-8C0F-742D892061F6}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{975C68A7-312C-419F-B597-E1BE3D93A92A}" name="Solution" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3515ED47-3F4E-4C8F-9977-604523CC8817}" name="Table2" displayName="Table2" ref="A1:H13" totalsRowShown="0" dataDxfId="18">
+  <autoFilter ref="A1:H13" xr:uid="{45544F43-3305-42C2-B8A6-EE9756F40048}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{8F49D62D-E299-4799-8741-D3D0E467E298}" name="Task"/>
+    <tableColumn id="2" xr3:uid="{CB82EEB2-6795-4473-9DF2-8E6771815F0A}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{09BF5DA9-DC53-44BE-A95E-E5E8BC918932}" name="Expectation" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{1F8C2F94-E69D-44EE-A126-8C397CA9C686}" name="Working Initially on Installable?" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{FA5A0BB3-E881-4C81-9E45-92519E5A6138}" name="Working Initially on Standalone?" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{82C92FCE-CDA1-440C-A4D8-22534E1FF160}" name="Issue" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{8B807206-DF16-4735-99F8-0AE69D4E5228}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{67963608-5158-49F7-9C56-7941FD9C6992}" name="Solution" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07218983-6A6C-4FD4-8F01-A7CF8F4E3424}" name="Table3" displayName="Table3" ref="A1:H13" totalsRowShown="0">
+  <autoFilter ref="A1:H13" xr:uid="{9626228F-2338-400A-8E0F-F336DA4E2858}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{05D49874-8A42-4A9B-B327-5F9E8CDA8E2F}" name="Task" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{1CD58447-6F40-433B-893A-798C7E631DE8}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{C2D20CF6-F128-4A7C-AEDC-C46279297CB6}" name="Expectation" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{E85D24E8-C387-4E8B-B4DC-294183B71347}" name="Working Initially on Installable?"/>
+    <tableColumn id="5" xr3:uid="{C4B84B19-449F-4288-811F-E5BFC43D17BC}" name="Working Initially on Standalone?"/>
+    <tableColumn id="6" xr3:uid="{3F317C8F-7E13-4CC8-AF2C-751AFE18C18E}" name="Issue"/>
+    <tableColumn id="7" xr3:uid="{52FD11AF-2D4C-4D01-AB35-BC53D4CABD00}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{FE6C481A-CD41-4558-B710-84686D7BFBD4}" name="Solution"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6C6C4F5C-D5DF-46EB-AB4A-CCF7B443D011}" name="Table4" displayName="Table4" ref="A1:H7" totalsRowShown="0">
+  <autoFilter ref="A1:H7" xr:uid="{E24F069B-A25B-4D04-82C2-439832F8CBC6}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{29998848-7BCD-4499-B61B-378AF411B8A8}" name="Task" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{98885AF8-3E75-4BF8-80CD-D8CEBC202B1C}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{1270836A-FA95-4E6C-A9F9-83554939CCF4}" name="Expectation" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{D3D13A95-CE79-47BD-8F20-F41CB555C00D}" name="Working initially on Installable?"/>
+    <tableColumn id="5" xr3:uid="{0B34E98D-3854-40FA-B1B2-EBA96D1F5EAF}" name="Working Initially on Standalone?"/>
+    <tableColumn id="6" xr3:uid="{99E7FF66-CA45-4208-B53E-5F61248C7289}" name="Issue"/>
+    <tableColumn id="7" xr3:uid="{00A38E54-4FEF-4D7B-9A46-A74F778CF515}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{0014E8CA-9192-43C7-B9BD-2CDC3F297E1F}" name="Solution"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8A4E3ECE-A2A6-4403-843E-F431F09F9EB4}" name="Table5" displayName="Table5" ref="A1:H10" totalsRowShown="0">
+  <autoFilter ref="A1:H10" xr:uid="{D4EDE50C-4B1F-431E-BAEA-02C9BE16D5B5}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{86B1B6B4-E6F8-4C3E-8ECF-1AA4DA9CD195}" name="Task" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{4AFDD15E-E863-4FFD-AD94-537766B1E317}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{C0B58DDD-27D3-432A-9F4A-9B764C1F1E89}" name="Expectation" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{1B901D77-5582-4D5F-9882-50D6D00B400E}" name="Working Initially on Installable?"/>
+    <tableColumn id="5" xr3:uid="{50532394-3441-4926-9502-615C39577634}" name="Working Initially on Standalone?"/>
+    <tableColumn id="6" xr3:uid="{13401DEC-EE3A-4D7D-B52F-032B1D5A40A0}" name="Issue"/>
+    <tableColumn id="7" xr3:uid="{77343F9D-21EE-4426-89D9-C3EC79B7B3CA}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{7ABF2BC5-F738-4BA7-8182-92A0170A7A0A}" name="Solution"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{38B70F0E-3D8D-4C12-A3DE-241EE20053C3}" name="Table6" displayName="Table6" ref="A1:H8" totalsRowShown="0">
+  <autoFilter ref="A1:H8" xr:uid="{BAEAFF49-E84D-4400-BF4D-091E7C13CAEC}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{3865FE8D-DBCE-4905-A9FA-E93E6063CF5F}" name="Task" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{2ABE7530-231B-4354-9D23-53A2A7442853}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{5337CC4F-8D73-4D94-B85D-4568BEDC0DF6}" name="Expectation" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{0C1896A2-F3DB-4674-8EB7-54B1FE6B3C3D}" name="Working Initially on Installable?" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{63F348AC-7F90-4EAD-957D-ACC8028A5573}" name="Working Initially on Standalone?" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{8F09D566-1E08-4B0B-8CBF-FBD0A806A184}" name="Issue"/>
+    <tableColumn id="7" xr3:uid="{D8AAE8F2-0356-47E9-8DBF-497EEC54C7DA}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{3CB713AF-1F83-4FA3-BD9B-923822E54F07}" name="Solution"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{85095D47-C8BD-4F91-A6DE-3C2AA465760C}" name="Table7" displayName="Table7" ref="A1:H5" totalsRowShown="0">
+  <autoFilter ref="A1:H5" xr:uid="{D7F91948-2EAA-43A7-BF15-BDC90B743FF0}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{75A90156-9335-41F9-A3A7-49836183A781}" name="Task" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{453ABDFA-C289-4955-A2C9-6DCBDAE0FA37}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{0EB173F7-1AD6-4381-AA64-DA20EA7ACDD2}" name="Expectation" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{B49DF1DB-9625-4B64-944F-B89C0AD8F3B9}" name="Working Initially on Installable?"/>
+    <tableColumn id="5" xr3:uid="{5A234A3A-9B0E-4A00-8637-8E56327BEC9B}" name="Working Initially on Standalone?"/>
+    <tableColumn id="6" xr3:uid="{722E6FD4-93EF-4022-8956-D2FF84D9AF4A}" name="Issue"/>
+    <tableColumn id="7" xr3:uid="{9608F234-F3D0-43B0-99A5-5012A81DB2C7}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{5B5A780F-A074-4AF0-8980-88F7331D66E5}" name="Solution"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7E1D93DC-2EAA-41A6-9F9C-D6A59F280EEF}" name="Table8" displayName="Table8" ref="A1:H13" totalsRowShown="0">
+  <autoFilter ref="A1:H13" xr:uid="{CE544966-9979-492E-BD92-2445BFEA035D}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{DFC3C427-D403-42E0-BADD-7DD37808B424}" name="Task" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A0C2820C-6D88-488C-B844-5806524A7F05}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{B930C9F2-5B29-450B-89A0-3D623D8C2390}" name="Expectation" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A2F18EFA-61D3-4E6D-B983-FBE4000F7D3A}" name="Working Initially on Installable?"/>
+    <tableColumn id="5" xr3:uid="{B58A5696-4A3C-45D9-B25C-8BF16859995A}" name="Working Initially on Standalone?"/>
+    <tableColumn id="6" xr3:uid="{3B7B5FA9-4AAD-4D8D-9F54-E39F5CE23B62}" name="Issue" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{2AF64310-00DC-49E7-BD11-222A10D8BE28}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{74796A4F-C180-4D68-84C3-B9833289598B}" name="Solution" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{092F5E4A-3933-4244-8246-80BE7A78C778}" name="Table9" displayName="Table9" ref="A1:H7" totalsRowShown="0">
+  <autoFilter ref="A1:H7" xr:uid="{51C7C2A6-472C-4599-9A46-42176831756C}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D8A00F48-445D-43E1-8F7D-E12BE2525788}" name="Task" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{9CA7F94E-3048-424C-A6B1-3C2648BAF154}" name="Control type"/>
+    <tableColumn id="3" xr3:uid="{11029337-B5D5-4D22-9AE5-47C278DC539D}" name="Expectation" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{DE193F2C-211C-46BA-9089-CA467E3F04F7}" name="Working Initially on Installable?"/>
+    <tableColumn id="5" xr3:uid="{A8708148-4F5E-4D96-B2CF-7DA65C559DE6}" name="Working Initially on Standalone?"/>
+    <tableColumn id="6" xr3:uid="{3264AD03-ED2E-4604-ADD1-79743BC1C7DA}" name="Issue"/>
+    <tableColumn id="7" xr3:uid="{EE484079-95AD-404B-8F65-3F14BDDE77A1}" name="Working now?"/>
+    <tableColumn id="8" xr3:uid="{3E90455D-41F1-4541-94BD-3C841E541085}" name="Solution"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -819,17 +1063,18 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="58.85546875" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="40.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1168,6 +1413,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1175,18 +1424,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFD59F2-CD4A-4263-87EF-57061A682B8C}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1516,6 +1766,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1523,19 +1777,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34EF0C79-979C-44B1-9657-30850D0404E5}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.85546875" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
     <col min="6" max="6" width="38.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="55.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1564,8 +1819,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
@@ -1590,8 +1845,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B3" t="s">
@@ -1607,8 +1862,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B4" t="s">
@@ -1624,8 +1879,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B5" t="s">
@@ -1641,8 +1896,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B6" t="s">
@@ -1658,8 +1913,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B7" t="s">
@@ -1676,7 +1931,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B8" t="s">
@@ -1692,8 +1947,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B9" t="s">
@@ -1709,8 +1964,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B10" t="s">
@@ -1726,8 +1981,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B11" t="s">
@@ -1743,8 +1998,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B12" t="s">
@@ -1760,8 +2015,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B13" t="s">
@@ -1779,6 +2034,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1787,17 +2046,18 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1974,6 +2234,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1982,17 +2246,18 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.42578125" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="6" max="6" width="42.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2198,6 +2463,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2206,16 +2475,18 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F9:F10"/>
+      <selection sqref="A1:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.42578125" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2397,6 +2668,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2405,15 +2680,19 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.28515625" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2512,6 +2791,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2520,16 +2803,19 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.28515625" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2777,6 +3063,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2784,19 +3074,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789B48B5-A7F7-4150-9633-D1931311379B}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.85546875" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2929,5 +3220,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>